<commit_message>
add Statistics by cities
</commit_message>
<xml_diff>
--- a/3.4 Pandas/report.xlsx
+++ b/3.4 Pandas/report.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -63,10 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -817,4 +819,231 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Город</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Уровень зарплат</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Город</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Доля вакансий</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>40201</v>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.334026018899322</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>38461</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.1014048968812217</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Новосибирск</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>34765</v>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Минск</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.04061388562982566</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Екатеринбург</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>32600</v>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Киев</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.03216914223228148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Краснодар</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>31798</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Новосибирск</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.02363188261188267</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Казань</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>29840</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Нижний Новгород</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.02144437701366958</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Ростов-на-Дону</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>28090</v>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Екатеринбург</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.01972705996450027</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Пермь</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>27517</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Алматы</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.01892116268106615</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Самара</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>27097</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Воронеж</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.01859600619490592</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Нижний Новгород</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>26376</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Казань</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.01856606725806701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>